<commit_message>
Annexe 18 tableau de calcul de coût
</commit_message>
<xml_diff>
--- a/client/public/fichiers/ANNEXE 18 - TABLEAU CALCUL DE COUT.xlsx
+++ b/client/public/fichiers/ANNEXE 18 - TABLEAU CALCUL DE COUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://219295cocerto-my.sharepoint.com/personal/lgombaud_cocerto_fr/Documents/SAUVEGARDE LOCAL LG/MEMOIRE DEC/MEMOIRE/ANNEXE/ANNEXE 18 - TABLEAU CALCUL DE COUT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgombaud\Documents\DEF MEMOIRE\ANNEXES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{9461C862-B0F5-4249-AC05-E3EC29721622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{287B892D-E390-41C7-86DB-4AB6698879FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F53A90-4F54-4266-B680-2615922D90F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{E763F31E-31DD-4C0D-91DE-0AF7FFD6452D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E763F31E-31DD-4C0D-91DE-0AF7FFD6452D}"/>
   </bookViews>
   <sheets>
     <sheet name="📘 Notice" sheetId="7" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'👤 Coût élève'!$A$1:$C$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'💰 Coût total'!$A$1:$G$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'📊 Données comptables'!$A$1:$G$82</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'📌 Indicateurs de pilotage '!$A$1:$C$27</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'📘 Notice'!$A$1:$A$117</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'📌 Indicateurs de pilotage '!$A$1:$C$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'📘 Notice'!$A$1:$A$115</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="235">
   <si>
     <t>NOTICE</t>
   </si>
@@ -145,7 +145,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">L’activation des </t>
+      <t xml:space="preserve">Les cases de </t>
     </r>
     <r>
       <rPr>
@@ -155,21 +155,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>macros</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> est nécessaire au bon fonctionnement de l’outil</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Les cases de </t>
+      <t>couleurs jaune clair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sont les seules à devoir être complétées, le reste du tableau est </t>
     </r>
     <r>
       <rPr>
@@ -179,16 +174,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>couleurs jaune clair</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sont les seules à devoir être complétées, le reste du tableau est </t>
+      <t>automatisé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le fichier est </t>
     </r>
     <r>
       <rPr>
@@ -198,7 +198,269 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>automatisé</t>
+      <t>protégé sans mot de passe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Il peut être adapté à d’autres projets en personnalisant les intitulés ou les hypothèses. Il est conseillé de dupliquer l’original avant toute modification</t>
+    </r>
+  </si>
+  <si>
+    <t>🎯 Objectif de l’annexe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L’Annexe 18 est un outil de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>calcul automatisé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> conçu pour exploiter les données issues du </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>plan comptable adapté</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (cf. Annexe 4) et fournir une analyse détaillée des coûts de l’école de production.</t>
+    </r>
+  </si>
+  <si>
+    <t>Elle permet de :</t>
+  </si>
+  <si>
+    <r>
+      <t>• Importer et consolider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> les données comptables filtrées depuis le plan comptable adapté, en intégrant uniquement les comptes de charges (classe 6) et de produits (classe 7) pertinents.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• Traiter automatiquement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> la ventilation des charges et produits </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>déjà sectorisés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> dans le plan comptable adapté entre :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">▫ secteur </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Production (T)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : activités génératrices de recettes soumises à TVA,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">▫ secteur </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pédagogie (NT)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : activités de formation exonérées,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">▫ secteur </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mutualisé (M)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : charges communes à répartir.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• Calculer le coût total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> par secteur, avec distinction claire entre activité de production et activité pédagogique, en intégrant charges directes et clé de répartition appliquée aux charges mutualisées.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• Établir le coût moyen par élève</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, basé sur les effectifs et hypothèses saisies, pour disposer d’un indicateur de suivi et de comparaison.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>• Produire des indicateurs de pilotage synthétiques</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, exploitables pour :</t>
+    </r>
+  </si>
+  <si>
+    <t>▫ analyser l’évolution des coûts,</t>
+  </si>
+  <si>
+    <t>▫ justifier l’utilisation des ressources,</t>
+  </si>
+  <si>
+    <t>▫ appuyer les échanges avec financeurs et partenaires.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">💡 Cet outil assure une </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>exploitation fiable et standardisée</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> des données comptables, garantissant la cohérence avec la structure définie dans l’Annexe 4 et facilitant la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>prise de décision stratégique</t>
     </r>
     <r>
       <rPr>
@@ -211,8 +473,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Le fichier est </t>
+    <t>🧱 Construction de l’outil</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L’Annexe 18 est composée de </t>
     </r>
     <r>
       <rPr>
@@ -222,24 +487,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>protégé sans mot de passe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>. Il peut être adapté à d’autres projets en personnalisant les intitulés ou les hypothèses. Il est conseillé de dupliquer l’original avant toute modification</t>
-    </r>
-  </si>
-  <si>
-    <t>🎯 Objectif de l’annexe</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L’Annexe 18 est un outil de </t>
+      <t>quatre onglets principaux</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Permet de saisir ou d’importer les données issues de la comptabilité, selon la nomenclature du </t>
     </r>
     <r>
       <rPr>
@@ -249,16 +511,27 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>calcul automatisé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> conçu pour exploiter les données issues du </t>
+      <t>plan comptable adapté</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Annexe 4).</t>
+    </r>
+  </si>
+  <si>
+    <t>• Budget Année N : à compléter une seule fois en début d’exercice.</t>
+  </si>
+  <si>
+    <t>• Saisie trimestrielle : chaque trimestre, reporter les montants de la balance comptable (exemple : Si l’exercice clôture au 31/08, le T1 correspond à la période du 01/09/N au 30/11/N).</t>
+  </si>
+  <si>
+    <r>
+      <t>Les comptes sont automatiquement classés par secteur d’activité (</t>
     </r>
     <r>
       <rPr>
@@ -268,47 +541,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>plan comptable adapté</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (cf. Annexe 4) et fournir une analyse détaillée des coûts de l’école de production.</t>
-    </r>
-  </si>
-  <si>
-    <t>Elle permet de :</t>
-  </si>
-  <si>
-    <r>
-      <t>• Importer et consolider</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> les données comptables filtrées depuis le plan comptable adapté, en intégrant uniquement les comptes de charges (classe 6) et de produits (classe 7) pertinents.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>• Traiter automatiquement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> la ventilation des charges et produits </t>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -318,21 +560,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>déjà sectorisés</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> dans le plan comptable adapté entre :</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">▫ secteur </t>
+      <t>NT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -342,154 +579,233 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Production (T)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : activités génératrices de recettes soumises à TVA,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">▫ secteur </t>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>) selon leur codification.</t>
+    </r>
+  </si>
+  <si>
+    <t>Suivi et indicateurs :</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• La colonne </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pédagogie (NT)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : activités de formation exonérées,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">▫ secteur </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Réel cumulé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> agrège automatiquement les montants saisis trimestre par trimestre.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Les colonnes </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Mutualisé (M)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : charges communes à répartir.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>• Calculer le coût total</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> par secteur, avec distinction claire entre activité de production et activité pédagogique, en intégrant charges directes et clé de répartition appliquée aux charges mutualisées.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>• Établir le coût moyen par élève</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>, basé sur les effectifs et hypothèses saisies, pour disposer d’un indicateur de suivi et de comparaison.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>• Produire des indicateurs de pilotage synthétiques</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, exploitables pour :</t>
-    </r>
-  </si>
-  <si>
-    <t>▫ analyser l’évolution des coûts,</t>
-  </si>
-  <si>
-    <t>▫ justifier l’utilisation des ressources,</t>
-  </si>
-  <si>
-    <t>▫ appuyer les échanges avec financeurs et partenaires.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">💡 Cet outil assure une </t>
+      <t>Écart (€)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>exploitation fiable et standardisée</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> des données comptables, garantissant la cohérence avec la structure définie dans l’Annexe 4 et facilitant la </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Écart (%)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> permettent de mesurer l’avancement de chaque ligne par rapport au budget annuel.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Un </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>prise de décision stratégique</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>code couleur automatique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> signale visuellement les écarts :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">▫ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour un dépassement de prévisions de produits.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">▫ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Rouge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour un dépassement de budget sur les charges.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cet onglet agrège l’ensemble des données par secteur — </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Production, Pédagogie et Mutualisé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> — afin de calculer automatiquement les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>charges directes de production</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>charges directes pédagogiques</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>charges mutualisées</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -497,100 +813,94 @@
     </r>
   </si>
   <si>
-    <t>🧱 Construction de l’outil</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L’Annexe 18 est composée de </t>
+    <r>
+      <t xml:space="preserve">Ces dernières sont ventilées de façon automatique selon une </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>quatre onglets principaux</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Permet de saisir ou d’importer les données issues de la comptabilité, selon la nomenclature du </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clé de répartition prédéfinie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>plan comptable adapté</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (Annexe 4).</t>
-    </r>
-  </si>
-  <si>
-    <t>• Budget Année N : à compléter une seule fois en début d’exercice.</t>
-  </si>
-  <si>
-    <r>
-      <t>Les comptes sont automatiquement classés par secteur d’activité (</t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2/3 pour l’activité de production et 1/3 pour l’activité pédagogique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, cette proportion étant fondée sur le temps passé et l’utilisation effective des ressources dans chaque secteur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le tableau fournit également une </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>synthèse claire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> permettant d’identifier le poids relatif de chaque secteur dans le </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>budget global</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et de visualiser leur évolution dans le temps.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L’onglet « Coût élève » présente un récapitulatif automatique des </t>
     </r>
     <r>
       <rPr>
@@ -600,24 +910,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>) selon leur codification.</t>
-    </r>
-  </si>
-  <si>
-    <t>Suivi et indicateurs :</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• La colonne </t>
+      <t>coûts d'un élève par secteur d’activité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il convient au préalable de compléter les </t>
     </r>
     <r>
       <rPr>
@@ -627,7 +934,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Réel cumulé</t>
+      <t>hypothèses clés retenues</t>
     </r>
     <r>
       <rPr>
@@ -636,12 +943,15 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> agrège automatiquement les montants saisis trimestre par trimestre.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• Les colonnes </t>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Les données sont déclinées en :</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• </t>
     </r>
     <r>
       <rPr>
@@ -651,12 +961,185 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Écart (€)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
+      <t>Coût total par élève</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour la production, la pédagogie et l’ensemble de l’école.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Coût horaire par élève</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, calculé selon le volume horaire consacré à chaque secteur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ces indicateurs sont affichés en</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Budget Annuel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Réel Cumulé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, avec un suivi des écarts entre ces deux données pour le coût horaire (Seule donnée comparable si les 4 trimestres ne sont pas complétées)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cet onglet regroupe automatiquement les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>indicateurs clés de performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> de l’école, calculés à partir des données saisies dans les onglets précédents.</t>
+    </r>
+  </si>
+  <si>
+    <t>Il présente notamment :</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Le </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>chiffre d’affaires total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et le </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>chiffre d’affaires par élève</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>charges externes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -666,49 +1149,159 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Écart (%)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> permettent de mesurer l’avancement de chaque ligne par rapport au budget annuel.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• Un </t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>charges de personnel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> totales.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Le </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>code couleur automatique</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> signale visuellement les écarts :</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">▫ </t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>seuil de rentabilité de l’activité de production</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, exprimé en euros de chiffre d’affaires à atteindre.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• La </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>marge brute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>marge nette</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sur l’activité de production, ainsi que leur pourcentage.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les données sont affichées en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Budget Annuel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Réel Cumulé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, avec calcul automatique des écarts en valeur et en pourcentage d’avancement.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>code couleur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> facilite la lecture :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• </t>
     </r>
     <r>
       <rPr>
@@ -722,16 +1315,16 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pour un dépassement de prévisions de produits.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">▫ </t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : performance ou économie favorable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• </t>
     </r>
     <r>
       <rPr>
@@ -745,611 +1338,21 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pour un dépassement de budget sur les charges.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cet onglet agrège l’ensemble des données par secteur — </t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : écart négatif ou dépassement.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cet onglet permet ainsi de </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Production, Pédagogie et Mutualisé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> — afin de calculer automatiquement les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>charges directes de production</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>charges directes pédagogiques</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>charges mutualisées</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ces dernières sont ventilées de façon automatique selon une </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>clé de répartition prédéfinie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2/3 pour l’activité de production et 1/3 pour l’activité pédagogique</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, cette proportion étant fondée sur le temps passé et l’utilisation effective des ressources dans chaque secteur.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le tableau fournit également une </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>synthèse claire</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> permettant d’identifier le poids relatif de chaque secteur dans le </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>budget global</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et de visualiser leur évolution dans le temps.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">L’onglet « Coût élève » présente un récapitulatif automatique des </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>coûts d'un élève par secteur d’activité</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Les données sont déclinées en :</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Coût total par élève</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pour la production, la pédagogie et l’ensemble de l’école.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Coût horaire par élève</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, calculé selon le volume horaire consacré à chaque secteur.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ces indicateurs sont affichés en</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Budget Annuel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et en </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Réel Cumulé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, avec un suivi des écarts entre ces deux données pour le coût horaire (Seule donnée comparable si les 4 trimestres ne sont pas complétées)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cet onglet regroupe automatiquement les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>indicateurs clés de performance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> de l’école, calculés à partir des données saisies dans les onglets précédents.</t>
-    </r>
-  </si>
-  <si>
-    <t>Il présente notamment :</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• Le </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>chiffre d’affaires total</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et le </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>chiffre d’affaires par élève</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• Les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>charges externes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>charges de personnel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> totales.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• Le </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>seuil de rentabilité de l’activité de production</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, exprimé en euros de chiffre d’affaires à atteindre.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• La </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>marge brute</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>marge nette</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sur l’activité de production, ainsi que leur pourcentage.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Les données sont affichées en </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Budget Annuel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et en </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Réel Cumulé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, avec calcul automatique des écarts en valeur et en pourcentage d’avancement.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Un </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>code couleur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> facilite la lecture :</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Vert</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : performance ou économie favorable.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Rouge</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : écart négatif ou dépassement.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cet onglet permet ainsi de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1367,7 +1370,7 @@
     </r>
   </si>
   <si>
-    <t>Données comptables</t>
+    <t>DONNEES COMPTABLES</t>
   </si>
   <si>
     <t>Compte</t>
@@ -1400,6 +1403,18 @@
     <t>Écart (%)</t>
   </si>
   <si>
+    <t>T - Achats matières premières - Production</t>
+  </si>
+  <si>
+    <t>T - Variation stock matière première - Production</t>
+  </si>
+  <si>
+    <t>M - Variation stock fourniture de bureau et d'entretien - Mutualisé</t>
+  </si>
+  <si>
+    <t>T - Sous-traitance technique - Production</t>
+  </si>
+  <si>
     <t>M - Électricité</t>
   </si>
   <si>
@@ -1526,9 +1541,21 @@
     <t>M - Cotisations syndicales et autres</t>
   </si>
   <si>
+    <t>M - Taxe sur les salaires - Mutualisé</t>
+  </si>
+  <si>
+    <t>NT - Taxe sur les salaires - Pédagogique</t>
+  </si>
+  <si>
+    <t>T - Taxe sur les salaires - Production</t>
+  </si>
+  <si>
     <t>M - Taxe d’apprentissage - Mutualisé</t>
   </si>
   <si>
+    <t>T - Taxe d’apprentissage - Production</t>
+  </si>
+  <si>
     <t>M - Formation continue - Mutualisé</t>
   </si>
   <si>
@@ -1616,7 +1643,10 @@
     <t>Produits d'exploitation cumulés</t>
   </si>
   <si>
-    <t>Calcul du coût total</t>
+    <t>CALCUL DU COUT TOTAL</t>
+  </si>
+  <si>
+    <t>Catégorie de charge de fonctionnement</t>
   </si>
   <si>
     <t>Budget Annuel (€)</t>
@@ -1733,25 +1763,25 @@
     <t>Calcul : Coût total production + Coût total pédagogie</t>
   </si>
   <si>
-    <t>Calcul du coût élève</t>
+    <t>CALCUL DU COUT ELEVE</t>
   </si>
   <si>
     <t>Hypothèses clés retenues</t>
   </si>
   <si>
-    <t>Nombre d'élèves total</t>
-  </si>
-  <si>
-    <t>Nombre de semaines d'enseignement/production par an</t>
-  </si>
-  <si>
-    <t>Nombre d'heures élève/semaine en atelier</t>
-  </si>
-  <si>
-    <t>Nombre d'heures élève/semaine en matières générales</t>
-  </si>
-  <si>
-    <t>Taux de marge brute théorique sur production</t>
+    <t>Nombre d'élèves total (Ex : 28)</t>
+  </si>
+  <si>
+    <t>Nombre de semaines d'enseignement/production par an (Ex : 42)</t>
+  </si>
+  <si>
+    <t>Nombre d'heures élève/semaine en atelier (Ex : 24)</t>
+  </si>
+  <si>
+    <t>Nombre d'heures élève/semaine en matières générales (Ex : 11)</t>
+  </si>
+  <si>
+    <t>Taux de marge brute théorique sur production (Ex : 60%)</t>
   </si>
   <si>
     <t>Coût global élève</t>
@@ -1806,7 +1836,22 @@
     <t>Calcul : Coût Total École/(Nombre d'élèves*Nb semaines*(Nb heures atelier+Nb heures matières générales))</t>
   </si>
   <si>
-    <t>Indicateurs de pilotage</t>
+    <t>INDICATEURS DE PILOTAGE</t>
+  </si>
+  <si>
+    <t>Nombre d'élèves total</t>
+  </si>
+  <si>
+    <t>Nombre de semaines d'enseignement/production par an</t>
+  </si>
+  <si>
+    <t>Nombre d'heures élève/semaine en atelier</t>
+  </si>
+  <si>
+    <t>Nombre d'heures élève/semaine en matières générales</t>
+  </si>
+  <si>
+    <t>Taux de marge brute théorique sur production</t>
   </si>
   <si>
     <t>Indicateurs</t>
@@ -1849,12 +1894,18 @@
     <t>Seuil de rentabilité de l'activité production</t>
   </si>
   <si>
-    <t>Charges prod. / Taux de marge de production</t>
-  </si>
-  <si>
     <t>Marge brute sur activité de production</t>
   </si>
   <si>
+    <t>Chiffre d’affaires - (achats matières premières + variation de stock matières + sous traitance production)</t>
+  </si>
+  <si>
+    <t>% de marge brute sur activité de production</t>
+  </si>
+  <si>
+    <t>Marge brute sur activité de production / Chiffre d'affaires</t>
+  </si>
+  <si>
     <t>Marge nette sur activité de production</t>
   </si>
   <si>
@@ -1867,82 +1918,7 @@
     <t>Marge nette sur activité de production / Chiffre d'affaires</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Il convient au préalable de compléter les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>hypothèses clés retenues</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Nombre d'élèves total (Ex : 28)</t>
-  </si>
-  <si>
-    <t>Nombre de semaines d'enseignement/production par an (Ex : 42)</t>
-  </si>
-  <si>
-    <t>Nombre d'heures élève/semaine en atelier (Ex : 24)</t>
-  </si>
-  <si>
-    <t>Nombre d'heures élève/semaine en matières générales (Ex : 11)</t>
-  </si>
-  <si>
-    <t>Taux de marge brute théorique sur production (Ex : 60%)</t>
-  </si>
-  <si>
-    <t>M - Taxe sur les salaires - Mutualisé</t>
-  </si>
-  <si>
-    <t>NT - Taxe sur les salaires - Pédagogique</t>
-  </si>
-  <si>
-    <t>T - Taxe sur les salaires - Production</t>
-  </si>
-  <si>
-    <t>T - Taxe d’apprentissage - Production</t>
-  </si>
-  <si>
-    <t>T - Achats matières premières - Production</t>
-  </si>
-  <si>
-    <t>T - Variation stock matière première - Production</t>
-  </si>
-  <si>
-    <t>M - Variation stock fourniture de bureau et d'entretien - Mutualisé</t>
-  </si>
-  <si>
-    <t>T - Sous-traitance technique - Production</t>
-  </si>
-  <si>
-    <t>Chiffre d’affaires - (achats matières premières + variation de stock matières + sous traitance production)</t>
-  </si>
-  <si>
-    <t>% de marge brute sur activité de production</t>
-  </si>
-  <si>
-    <t>Marge brute sur activité de production / Chiffre d'affaires</t>
-  </si>
-  <si>
-    <t>• Saisie trimestrielle : chaque trimestre, reporter les montants de la balance comptable (exemple : Si l’exercice clôture au 31/08, le T1 correspond à la période du 01/09/N au 30/11/N).</t>
-  </si>
-  <si>
-    <t>Catégorie de charge de fonctionnement</t>
+    <t>Coût total de l'activité de production / Taux de marge de production</t>
   </si>
 </sst>
 </file>
@@ -2535,13 +2511,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1981427</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>9558</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2579,13 +2555,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1286005</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>190532</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2623,13 +2599,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1305058</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>181006</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2667,13 +2643,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2076689</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>190531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3031,9 +3007,9 @@
     <tabColor rgb="FFC9D7F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A117"/>
+  <dimension ref="A1:A115"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3095,68 +3071,68 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="48"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="49" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-    </row>
-    <row r="19" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A18" s="33"/>
+    </row>
+    <row r="19" spans="1:1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
     </row>
-    <row r="21" spans="1:1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-    </row>
-    <row r="23" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+    </row>
+    <row r="25" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-    </row>
-    <row r="27" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
+      <c r="A28" s="35"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
+      <c r="A30" s="38"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
@@ -3172,39 +3148,39 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
+      <c r="A34" s="35"/>
+    </row>
+    <row r="35" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="37"/>
     </row>
     <row r="37" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="40" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-    </row>
-    <row r="39" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A38" s="40"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
+      <c r="A40" s="35"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="38" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="38"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="38" t="s">
@@ -3219,48 +3195,48 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+    <row r="47" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+    </row>
+    <row r="49" spans="1:1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-    </row>
-    <row r="51" spans="1:1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="50" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="33"/>
+    </row>
+    <row r="51" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
-    </row>
-    <row r="53" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+    <row r="52" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="41" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
+      <c r="A56" s="41"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="41"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="42"/>
+    </row>
+    <row r="59" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="42" t="s">
         <v>28</v>
       </c>
@@ -3268,33 +3244,33 @@
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="42"/>
     </row>
-    <row r="61" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="42" t="s">
-        <v>234</v>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="41" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="42"/>
+      <c r="A62" s="41"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
-        <v>30</v>
+      <c r="A65" s="42" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
+      <c r="A66" s="42"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
@@ -3302,65 +3278,65 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="42"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="42"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="42"/>
-    </row>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="37"/>
-    </row>
-    <row r="78" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="37"/>
+    </row>
+    <row r="76" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="36"/>
+    </row>
+    <row r="78" spans="1:1" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="36"/>
     </row>
-    <row r="80" spans="1:1" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
-    </row>
-    <row r="82" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="37"/>
+    </row>
+    <row r="83" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="39" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="84" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="37"/>
+      <c r="A84" s="36"/>
     </row>
     <row r="85" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -3368,7 +3344,7 @@
     </row>
     <row r="87" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="39" t="s">
-        <v>217</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -3376,48 +3352,48 @@
     </row>
     <row r="89" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="36"/>
+      <c r="A90" s="39"/>
     </row>
     <row r="91" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="39" t="s">
-        <v>41</v>
+      <c r="A91" s="36" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="39"/>
     </row>
-    <row r="93" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="39"/>
-    </row>
-    <row r="95" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="37"/>
+    </row>
+    <row r="96" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="97" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="37"/>
     </row>
-    <row r="98" spans="1:1" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" s="34" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="37"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
@@ -3425,7 +3401,7 @@
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
@@ -3433,7 +3409,7 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="37" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
@@ -3441,57 +3417,49 @@
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="37" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="37"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="37"/>
-    </row>
-    <row r="110" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="37" t="s">
-        <v>50</v>
-      </c>
+      <c r="A109" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="37"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="37"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="37"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A115" s="37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="37"/>
-    </row>
-    <row r="117" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="A15">
     <cfRule type="expression" dxfId="22" priority="33">
       <formula>ISNA(#REF!)</formula>
     </cfRule>
@@ -3502,7 +3470,7 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="50" max="16383" man="1"/>
+    <brk id="48" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3518,7 +3486,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69:G69"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,7 +3503,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -3549,34 +3517,34 @@
     </row>
     <row r="2" spans="1:10" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3584,7 +3552,7 @@
         <v>60100</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>227</v>
+        <v>67</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -3609,7 +3577,7 @@
         <v>60310</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>228</v>
+        <v>68</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -3634,7 +3602,7 @@
         <v>60320</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>229</v>
+        <v>69</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -3659,7 +3627,7 @@
         <v>60410</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>230</v>
+        <v>70</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -3684,7 +3652,7 @@
         <v>60611</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3709,7 +3677,7 @@
         <v>60626</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -3734,7 +3702,7 @@
         <v>60630</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -3759,7 +3727,7 @@
         <v>60632</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3784,7 +3752,7 @@
         <v>60631</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -3809,7 +3777,7 @@
         <v>60640</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3834,7 +3802,7 @@
         <v>60650</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3859,7 +3827,7 @@
         <v>60660</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -3884,7 +3852,7 @@
         <v>60690</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -3909,7 +3877,7 @@
         <v>61320</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -3934,7 +3902,7 @@
         <v>61340</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -3959,7 +3927,7 @@
         <v>61350</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -3984,7 +3952,7 @@
         <v>61360</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -4009,7 +3977,7 @@
         <v>61400</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -4034,7 +4002,7 @@
         <v>61520</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
@@ -4059,7 +4027,7 @@
         <v>61521</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -4084,7 +4052,7 @@
         <v>61522</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -4109,7 +4077,7 @@
         <v>61600</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -4134,7 +4102,7 @@
         <v>61830</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -4159,7 +4127,7 @@
         <v>62110</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -4184,7 +4152,7 @@
         <v>62111</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
@@ -4209,7 +4177,7 @@
         <v>62112</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -4234,7 +4202,7 @@
         <v>62260</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -4259,7 +4227,7 @@
         <v>62261</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -4284,7 +4252,7 @@
         <v>62270</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -4309,7 +4277,7 @@
         <v>62310</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
@@ -4334,7 +4302,7 @@
         <v>62320</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -4359,7 +4327,7 @@
         <v>62340</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -4384,7 +4352,7 @@
         <v>62410</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
@@ -4409,7 +4377,7 @@
         <v>62510</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -4434,7 +4402,7 @@
         <v>62520</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -4459,7 +4427,7 @@
         <v>62550</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -4484,7 +4452,7 @@
         <v>62560</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -4509,7 +4477,7 @@
         <v>62610</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -4534,7 +4502,7 @@
         <v>62620</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -4559,7 +4527,7 @@
         <v>62640</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -4584,7 +4552,7 @@
         <v>62680</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -4609,7 +4577,7 @@
         <v>62710</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -4634,7 +4602,7 @@
         <v>62810</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -4659,7 +4627,7 @@
         <v>62830</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -4684,7 +4652,7 @@
         <v>62840</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -4709,7 +4677,7 @@
         <v>62850</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -4734,7 +4702,7 @@
         <v>63110</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>223</v>
+        <v>113</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -4759,7 +4727,7 @@
         <v>63111</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>224</v>
+        <v>114</v>
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -4784,7 +4752,7 @@
         <v>63112</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>225</v>
+        <v>115</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -4809,7 +4777,7 @@
         <v>63120</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -4834,7 +4802,7 @@
         <v>63121</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -4859,7 +4827,7 @@
         <v>63330</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -4884,7 +4852,7 @@
         <v>63331</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -4909,7 +4877,7 @@
         <v>63332</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -4934,7 +4902,7 @@
         <v>63510</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
@@ -4959,7 +4927,7 @@
         <v>64110</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -4984,7 +4952,7 @@
         <v>64111</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -5009,7 +4977,7 @@
         <v>64112</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -5034,7 +5002,7 @@
         <v>64120</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -5059,7 +5027,7 @@
         <v>64121</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -5084,7 +5052,7 @@
         <v>64122</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
@@ -5109,7 +5077,7 @@
         <v>64510</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
@@ -5134,7 +5102,7 @@
         <v>64511</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
@@ -5159,7 +5127,7 @@
         <v>64512</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="18"/>
@@ -5184,7 +5152,7 @@
         <v>66110</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="18"/>
@@ -5209,7 +5177,7 @@
         <v>67800</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="18"/>
@@ -5232,7 +5200,7 @@
     <row r="69" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="27" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C69" s="23">
         <f>SUM(C3:C68)</f>
@@ -5272,7 +5240,7 @@
         <v>70600</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="18"/>
@@ -5297,7 +5265,7 @@
         <v>70601</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="18"/>
@@ -5322,7 +5290,7 @@
         <v>70602</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="18"/>
@@ -5347,7 +5315,7 @@
         <v>70620</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="18"/>
@@ -5372,7 +5340,7 @@
         <v>70700</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
@@ -5397,7 +5365,7 @@
         <v>70701</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="18"/>
@@ -5422,7 +5390,7 @@
         <v>70702</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="18"/>
@@ -5447,7 +5415,7 @@
         <v>70720</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="18"/>
@@ -5472,7 +5440,7 @@
         <v>71331</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="18"/>
@@ -5497,7 +5465,7 @@
         <v>71335</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="18"/>
@@ -5522,7 +5490,7 @@
         <v>72210</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="18"/>
@@ -5547,7 +5515,7 @@
         <v>72220</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="18"/>
@@ -5570,7 +5538,7 @@
     <row r="82" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="27" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C82" s="23">
         <f>SUM(C70:C81)</f>
@@ -5708,9 +5676,9 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5725,7 +5693,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -5737,38 +5705,38 @@
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>235</v>
+        <v>148</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B5" s="7">
         <f>'📊 Données comptables'!C60+'📊 Données comptables'!C63+'📊 Données comptables'!C66+'📊 Données comptables'!C28</f>
@@ -5795,12 +5763,12 @@
         <v>0</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B6" s="7">
         <f>'📊 Données comptables'!C11+'📊 Données comptables'!C13+'📊 Données comptables'!C14+'📊 Données comptables'!C15+'📊 Données comptables'!C19+'📊 Données comptables'!C23</f>
@@ -5827,12 +5795,12 @@
         <v>0</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B7" s="7">
         <f>'📊 Données comptables'!C53+'📊 Données comptables'!C56+'📊 Données comptables'!C51</f>
@@ -5859,12 +5827,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B8" s="52">
         <f>SUM(B5:B7)</f>
@@ -5894,7 +5862,7 @@
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -5905,7 +5873,7 @@
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B10" s="7">
         <f>'📊 Données comptables'!C27+'📊 Données comptables'!C59+'📊 Données comptables'!C62+'📊 Données comptables'!C65</f>
@@ -5932,12 +5900,12 @@
         <v>0</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B11" s="7">
         <f>'📊 Données comptables'!C10+'📊 Données comptables'!C22+'📊 Données comptables'!C32+'📊 Données comptables'!C38+'📊 Données comptables'!C45+'📊 Données comptables'!C46+'📊 Données comptables'!C47</f>
@@ -5964,12 +5932,12 @@
         <v>0</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B12" s="7">
         <f>'📊 Données comptables'!C57+'📊 Données comptables'!C55+'📊 Données comptables'!C50</f>
@@ -5996,12 +5964,12 @@
         <v>0</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B13" s="52">
         <f t="shared" ref="B13:G13" si="1">SUM(B10:B12)</f>
@@ -6031,7 +5999,7 @@
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -6042,7 +6010,7 @@
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B15" s="7">
         <f>'📊 Données comptables'!C26+'📊 Données comptables'!C58+'📊 Données comptables'!C61+'📊 Données comptables'!C64</f>
@@ -6069,12 +6037,12 @@
         <v>0</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B16" s="7">
         <f>'📊 Données comptables'!C5+'📊 Données comptables'!C7+'📊 Données comptables'!C8+'📊 Données comptables'!C9+'📊 Données comptables'!C12+'📊 Données comptables'!C16+'📊 Données comptables'!C17+'📊 Données comptables'!C18+'📊 Données comptables'!C20+'📊 Données comptables'!C21+'📊 Données comptables'!C24+'📊 Données comptables'!C25+'📊 Données comptables'!C26+'📊 Données comptables'!C29+'📊 Données comptables'!C30+'📊 Données comptables'!C31+'📊 Données comptables'!C33+'📊 Données comptables'!C34+'📊 Données comptables'!C35+'📊 Données comptables'!C36+'📊 Données comptables'!C37+'📊 Données comptables'!C39+'📊 Données comptables'!C40+'📊 Données comptables'!C41+'📊 Données comptables'!C42+'📊 Données comptables'!C43+'📊 Données comptables'!C44+'📊 Données comptables'!C48</f>
@@ -6101,12 +6069,12 @@
         <v>0</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B17" s="7">
         <f>'📊 Données comptables'!C52+'📊 Données comptables'!C54+'📊 Données comptables'!C49</f>
@@ -6133,12 +6101,12 @@
         <v>0</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B18" s="7">
         <f>'📊 Données comptables'!C67+'📊 Données comptables'!C68</f>
@@ -6165,12 +6133,12 @@
         <v>0</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B19" s="52">
         <f t="shared" ref="B19:G19" si="2">SUM(B15:B18)</f>
@@ -6207,7 +6175,7 @@
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6226,7 +6194,7 @@
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B23" s="52">
         <f>B8+(B19*2/3)</f>
@@ -6253,7 +6221,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6267,7 +6235,7 @@
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B25" s="52">
         <f t="shared" ref="B25:G25" si="4">B13+(B19*1/3)</f>
@@ -6294,7 +6262,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,7 +6276,7 @@
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B27" s="52">
         <f t="shared" ref="B27:G27" si="5">B23+B25</f>
@@ -6335,7 +6303,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -6371,7 +6339,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="63"/>
@@ -6379,56 +6347,56 @@
     </row>
     <row r="2" spans="1:4" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="B3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="B4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="B5" s="58"/>
     </row>
     <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="B6" s="58"/>
     </row>
     <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="B7" s="57"/>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B11" s="7" t="str">
         <f>IF(B3=0,"",'💰 Coût total'!B23/B3)</f>
@@ -6441,7 +6409,7 @@
     </row>
     <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -6452,7 +6420,7 @@
     </row>
     <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B14" s="7" t="str">
         <f>IF(B3=0,"",'💰 Coût total'!B25/B3)</f>
@@ -6465,7 +6433,7 @@
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -6476,7 +6444,7 @@
     </row>
     <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B17" s="7" t="str">
         <f>IF(B3=0,"",'💰 Coût total'!B27/B3)</f>
@@ -6489,7 +6457,7 @@
     </row>
     <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6497,22 +6465,22 @@
     <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:4" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B22" s="52" t="str">
         <f>IF(B3=0,"",('💰 Coût total'!B23/(B3*B4*B5)))</f>
@@ -6529,7 +6497,7 @@
     </row>
     <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -6542,7 +6510,7 @@
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="B25" s="52" t="str">
         <f>IF(B3=0,"",('💰 Coût total'!B25/(B3*B4*B6)))</f>
@@ -6559,7 +6527,7 @@
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -6572,7 +6540,7 @@
     </row>
     <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="B28" s="52" t="str">
         <f>IF(B3=0,"",('💰 Coût total'!B27/(B3*B4*(B5+B6))))</f>
@@ -6589,7 +6557,7 @@
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6634,10 +6602,10 @@
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6652,7 +6620,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -6661,13 +6629,13 @@
     </row>
     <row r="2" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="B3" s="6">
         <f>'👤 Coût élève'!B3</f>
@@ -6676,7 +6644,7 @@
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="B4" s="6">
         <f>'👤 Coût élève'!B4</f>
@@ -6685,7 +6653,7 @@
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="B5" s="60">
         <f>'👤 Coût élève'!B5</f>
@@ -6694,7 +6662,7 @@
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="B6" s="60">
         <f>'👤 Coût élève'!B6</f>
@@ -6703,7 +6671,7 @@
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="B7" s="16">
         <f>'👤 Coût élève'!B7</f>
@@ -6713,25 +6681,24 @@
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B11" s="14">
         <f>'📊 Données comptables'!C82</f>
@@ -6751,9 +6718,9 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="B12" s="14">
         <f>'💰 Coût total'!B6+'💰 Coût total'!B11+'💰 Coût total'!B16</f>
@@ -6768,14 +6735,14 @@
         <v>0</v>
       </c>
       <c r="E12" s="11" t="str">
-        <f t="shared" ref="E12:E13" si="0">IF(B12=0,"",(C12/B12))</f>
+        <f t="shared" ref="E12:E15" si="0">IF(B12=0,"",(C12/B12))</f>
         <v/>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="B13" s="14">
         <f>'💰 Coût total'!B5+'💰 Coût total'!B10+'💰 Coût total'!B15</f>
@@ -6795,181 +6762,225 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="14">
+        <f>'💰 Coût total'!B23</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="14">
+        <f>'💰 Coût total'!G23</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" ref="D14:D15" si="1">C14-B14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>IF(B14=0,"",(C14/B14))</f>
+        <v/>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="B15" s="14">
-        <f>IF(B3=0,0,(('📊 Données comptables'!C82)/B3))</f>
+        <f>'💰 Coût total'!B25</f>
         <v>0</v>
       </c>
       <c r="C15" s="14">
-        <f>IF(B3=0,0,(('📊 Données comptables'!D82+'📊 Données comptables'!E82+'📊 Données comptables'!F82+'📊 Données comptables'!G82)/'📌 Indicateurs de pilotage '!B3))</f>
+        <f>'💰 Coût total'!G25</f>
         <v>0</v>
       </c>
       <c r="D15" s="14">
-        <f t="shared" ref="D15" si="1">C15-B15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="11" t="str">
-        <f>IF(C15=0,"",(C15/B15))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>209</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="B18" s="14">
-        <f>IF(B7=0,0,('💰 Coût total'!B23/'📌 Indicateurs de pilotage '!B7))</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="14">
-        <f>IF(B7=0,0,('💰 Coût total'!G23/'📌 Indicateurs de pilotage '!B7))</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="14">
-        <f>C18-B18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>211</v>
-      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="14">
+        <f>IF(B3=0,0,(('📊 Données comptables'!C82)/B3))</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="14">
+        <f>IF(B3=0,0,(('📊 Données comptables'!D82+'📊 Données comptables'!E82+'📊 Données comptables'!F82+'📊 Données comptables'!G82)/'📌 Indicateurs de pilotage '!B3))</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" ref="D17" si="2">C17-B17</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="11" t="str">
+        <f>IF(C17=0,"",(C17/B17))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="13"/>
     </row>
-    <row r="20" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="B21" s="14">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="14">
+        <f>IF(B7=0,0,('💰 Coût total'!B23/'📌 Indicateurs de pilotage '!B7))</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="14">
+        <f>IF(B7=0,0,('💰 Coût total'!G23/'📌 Indicateurs de pilotage '!B7))</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="14">
+        <f>C20-B20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="14">
         <f>B11*B7</f>
         <v>0</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C23" s="14">
         <f>(C11-('📊 Données comptables'!H3+'📊 Données comptables'!H4+'📊 Données comptables'!H6))</f>
         <v>0</v>
       </c>
-      <c r="D21" s="14">
-        <f>C21-B21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="D23" s="14">
+        <f>C23-B23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B26" s="16">
+        <f>IF(B11=0,0,(B23/B11))</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="16">
+        <f>IF(C11=0,0,(C23/C11))</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="16">
+        <f>C26-B26</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29" s="14">
+        <f>B23-'💰 Coût total'!B23</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="14">
+        <f>C23-'💰 Coût total'!G23</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="14">
+        <f>C29-B29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B24" s="16">
-        <f>IF(B11=0,0,(B21/B11))</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="16">
-        <f>IF(C11=0,0,(C21/C11))</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="16">
-        <f>C24-B24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="B32" s="16">
+        <f>IF(B11=0,0,(B29/B11))</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="16">
+        <f>IF(C11=0,0,(C29/C11))</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="16">
+        <f>C32-B32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
         <v>233</v>
-      </c>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="B27" s="14">
-        <f>B21-'💰 Coût total'!B23</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="14">
-        <f>C21-'💰 Coût total'!G23</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="14">
-        <f>C27-B27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B30" s="16">
-        <f>IF(B11=0,0,(B27/B11))</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="16">
-        <f>IF(C11=0,0,(C27/C11))</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="16">
-        <f>C30-B30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -6978,7 +6989,7 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B30:C30">
+  <conditionalFormatting sqref="B32:C32">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6986,7 +6997,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:D27">
+  <conditionalFormatting sqref="B29:D29">
     <cfRule type="cellIs" dxfId="13" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -6994,7 +7005,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D20">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7002,7 +7013,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D23">
     <cfRule type="cellIs" dxfId="9" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7010,7 +7021,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7018,15 +7029,15 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="D32">
     <cfRule type="expression" dxfId="5" priority="11">
-      <formula>$B$30&gt;$C$30</formula>
+      <formula>$B$32&gt;$C$32</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="12">
-      <formula>$C$30&gt;=$B$30</formula>
+      <formula>$C$32&gt;=$B$32</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11 E15">
+  <conditionalFormatting sqref="E11 E17">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -7034,7 +7045,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E13">
+  <conditionalFormatting sqref="E12:E15">
     <cfRule type="cellIs" dxfId="1" priority="35" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>